<commit_message>
Some tests might revert
</commit_message>
<xml_diff>
--- a/Zeus OS Workspace 2018 2.4/Zeus/data/TOP/Results/TOPPROB3-2-l.PRN.xlsx.2_short_HighestDemandInReachableArea.xlsx
+++ b/Zeus OS Workspace 2018 2.4/Zeus/data/TOP/Results/TOPPROB3-2-l.PRN.xlsx.2_short_HighestDemandInReachableArea.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="18">
   <si>
     <t xml:space="preserve">File: </t>
   </si>
@@ -50,19 +50,22 @@
     <t>Inital Solution 0 changes  totQ=800.00 totD=135.88 $135.88</t>
   </si>
   <si>
-    <t>Inital Solution 0 changes  totQ=800.00 totD=108.27 $108.27</t>
-  </si>
-  <si>
-    <t>Inital Solution 0 changes  totQ=800.00 totD=122.69 $122.69</t>
+    <t>Inital Solution 0 changes  totQ=800.00 totD=138.99 $138.99</t>
+  </si>
+  <si>
+    <t>Inital Solution 0 changes  totQ=800.00 totD=125.02 $125.02</t>
   </si>
   <si>
     <t>Inital Solution 0 changes  totQ=800.00 totD=107.32 $107.32</t>
   </si>
   <si>
+    <t>Inital Solution 0 changes  totQ=800.00 totD=110.97 $110.97</t>
+  </si>
+  <si>
     <t>Inital Solution 0 changes  totQ=800.00 totD=106.78 $106.78</t>
   </si>
   <si>
-    <t>Inital Solution 0 changes  totQ=800.00 totD=120.14 $120.14</t>
+    <t>Inital Solution 0 changes  totQ=800.00 totD=114.96 $114.96</t>
   </si>
 </sst>
 </file>
@@ -389,22 +392,22 @@
         <v>14</v>
       </c>
       <c r="T13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="U13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="V13" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="W13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="X13" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="Y13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>